<commit_message>
Feat : Update PPT
</commit_message>
<xml_diff>
--- a/220704/220704_user_분석.xlsx
+++ b/220704/220704_user_분석.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAMILY\Desktop\데이터 사이언티스트\EDA_Project\ll\lol_curse_winrate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hote\Desktop\Data Scientist Course\09.EDA Project\lol_curse_winrate\220704\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B2344-2033-4570-B6AF-9B5D5CA395B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE6801A-1405-471A-87FA-50BE0DBD754F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_비율" sheetId="1" r:id="rId1"/>
     <sheet name="User_승률" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="113">
   <si>
     <t>Unranked</t>
   </si>
@@ -248,6 +249,303 @@
   </si>
   <si>
     <t xml:space="preserve">Iron 2 </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>표본</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Grandmaster</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>challenger</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 데이터</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>표본 데이터</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>증감율</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Challenger</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill 총합</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Death 총합</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assist 총합</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임판수</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>표본 평균 Kill / Death / Assist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 평균 Kill / Death / Assist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 Data K/D/A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>W/L   mode</t>
+  </si>
+  <si>
+    <t>LOSS  솔로랭크    7813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      칼바람     2579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      일반      1238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      자유랭크    1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      URF      694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      단일       121</t>
+  </si>
+  <si>
+    <t>WIN   솔로랭크    7281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      칼바람     2567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      일반      1236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      자유랭크    1118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      URF      680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      단일       113</t>
+  </si>
+  <si>
+    <t>솔로랭크</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>칼바람</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유랭크</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>URF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>단일모드</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mode</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lose</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>승률</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>랭크게임</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반게임</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>스페셜게임</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Position  W/L </t>
+  </si>
+  <si>
+    <t>adc       LOSS    2713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          WIN     2665</t>
+  </si>
+  <si>
+    <t>jungle    LOSS    2890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          WIN     2825</t>
+  </si>
+  <si>
+    <t>mid       LOSS    2749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          WIN     2677</t>
+  </si>
+  <si>
+    <t>support   LOSS    2489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          WIN     2331</t>
+  </si>
+  <si>
+    <t>top       LOSS    2627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          WIN     2497</t>
+  </si>
+  <si>
+    <t>모드별 분석</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>포지션</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>분석</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>챔피언</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>분석</t>
+    </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -255,10 +553,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +750,19 @@
       <color theme="1"/>
       <name val="Rix모던고딕 B"/>
       <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -884,7 +1197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -914,6 +1227,30 @@
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1841,7 +2178,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>User_승률!$G$10:$G$16</c15:sqref>
@@ -1876,7 +2213,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>User_승률!$I$10:$I$16</c15:sqref>
@@ -1910,7 +2247,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1114-491F-83D3-16A9A39BAE1F}"/>
                   </c:ext>
@@ -1933,7 +2270,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>User_승률!$G$10:$G$16</c15:sqref>
@@ -1968,7 +2305,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>User_승률!$J$10:$J$16</c15:sqref>
@@ -2002,7 +2339,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-1114-491F-83D3-16A9A39BAE1F}"/>
                   </c:ext>
@@ -4212,11 +4549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="K17" sqref="J17:K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -4328,7 +4665,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25">
+    <row r="12" spans="1:7" ht="17.5">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -4340,7 +4677,7 @@
         <v>2.3383768913342505E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25">
+    <row r="13" spans="1:7" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -4353,7 +4690,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="17.25">
+    <row r="14" spans="1:7" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -4366,7 +4703,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="17.25">
+    <row r="15" spans="1:7" ht="17.5">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4379,7 +4716,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="17.25">
+    <row r="16" spans="1:7" ht="17.5">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -4392,7 +4729,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="17.25">
+    <row r="17" spans="1:17" ht="17.5">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -4413,7 +4750,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="17.25">
+    <row r="18" spans="1:17" ht="17.5">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -4434,7 +4771,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="17.25">
+    <row r="19" spans="1:17" ht="17.5">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -4455,7 +4792,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="17.25">
+    <row r="20" spans="1:17" ht="17.5">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -4481,7 +4818,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:17" ht="17.25">
+    <row r="21" spans="1:17" ht="17.5">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -4507,7 +4844,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:17" ht="17.25">
+    <row r="22" spans="1:17" ht="17.5">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -4533,7 +4870,7 @@
       <c r="M22" s="5"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:17" ht="17.25">
+    <row r="23" spans="1:17" ht="17.5">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -4559,7 +4896,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:17" ht="17.25">
+    <row r="24" spans="1:17" ht="17.5">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -4585,7 +4922,7 @@
       <c r="M24" s="5"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:17" ht="17.25">
+    <row r="25" spans="1:17" ht="17.5">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -4612,7 +4949,7 @@
       <c r="N25" s="2"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" ht="17.25">
+    <row r="26" spans="1:17" ht="17.5">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -4639,7 +4976,7 @@
       <c r="N26" s="2"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" ht="17.25">
+    <row r="27" spans="1:17" ht="17.5">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -4661,7 +4998,7 @@
       <c r="N27" s="2"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" ht="17.25">
+    <row r="28" spans="1:17" ht="17.5">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -4683,7 +5020,7 @@
       <c r="N28" s="2"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" ht="17.25">
+    <row r="29" spans="1:17" ht="17.5">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -4705,7 +5042,7 @@
       <c r="N29" s="2"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" ht="17.25">
+    <row r="30" spans="1:17" ht="17.5">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -4727,7 +5064,7 @@
       <c r="N30" s="2"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" ht="17.25">
+    <row r="31" spans="1:17" ht="17.5">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -4749,7 +5086,7 @@
       <c r="N31" s="2"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:17" ht="17.25">
+    <row r="32" spans="1:17" ht="17.5">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -4771,7 +5108,7 @@
       <c r="N32" s="2"/>
       <c r="Q32" s="4"/>
     </row>
-    <row r="33" spans="1:14" ht="17.25">
+    <row r="33" spans="1:14" ht="17.5">
       <c r="B33">
         <f>SUM(B12:B32)</f>
         <v>727</v>
@@ -4790,7 +5127,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" ht="17.25">
+    <row r="34" spans="1:14" ht="17.5">
       <c r="G34" s="6"/>
       <c r="J34" s="5" t="s">
         <v>24</v>
@@ -4801,7 +5138,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" ht="17.25">
+    <row r="35" spans="1:14" ht="17.5">
       <c r="J35" s="5" t="s">
         <v>25</v>
       </c>
@@ -4811,7 +5148,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" ht="17.25">
+    <row r="36" spans="1:14" ht="17.5">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -4831,7 +5168,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" ht="17.25">
+    <row r="37" spans="1:14" ht="17.5">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -4851,7 +5188,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" ht="17.25">
+    <row r="38" spans="1:14" ht="17.5">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -4871,7 +5208,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" ht="17.25">
+    <row r="39" spans="1:14" ht="17.5">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -4891,7 +5228,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="17.25">
+    <row r="40" spans="1:14" ht="17.5">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -4911,7 +5248,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" ht="17.25">
+    <row r="41" spans="1:14" ht="17.5">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -4925,7 +5262,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" ht="17.25">
+    <row r="42" spans="1:14" ht="17.5">
       <c r="B42">
         <v>727</v>
       </c>
@@ -4936,58 +5273,58 @@
       <c r="M42" s="5"/>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" ht="17.25">
+    <row r="43" spans="1:14" ht="17.5">
       <c r="M43" s="5"/>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" ht="17.25">
+    <row r="44" spans="1:14" ht="17.5">
       <c r="M44" s="5"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" ht="17.25">
+    <row r="45" spans="1:14" ht="17.5">
       <c r="M45" s="5"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" ht="17.25">
+    <row r="46" spans="1:14" ht="17.5">
       <c r="M46" s="5"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" ht="17.25">
+    <row r="47" spans="1:14" ht="17.5">
       <c r="M47" s="5"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" ht="17.25">
+    <row r="48" spans="1:14" ht="17.5">
       <c r="M48" s="5"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" ht="17.25">
+    <row r="49" spans="1:14" ht="17.5">
       <c r="M49" s="5"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" ht="17.25">
+    <row r="50" spans="1:14" ht="17.5">
       <c r="M50" s="5"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" ht="17.25">
+    <row r="51" spans="1:14" ht="17.5">
       <c r="M51" s="5"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" ht="17.25">
+    <row r="52" spans="1:14" ht="17.5">
       <c r="M52" s="5"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" ht="17.25">
+    <row r="53" spans="1:14" ht="17.5">
       <c r="M53" s="5"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" ht="17.25">
+    <row r="54" spans="1:14" ht="17.5">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="5"/>
       <c r="M54" s="5"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" ht="17.25">
+    <row r="55" spans="1:14" ht="17.5">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="5"/>
@@ -4995,7 +5332,7 @@
       <c r="M55" s="5"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" ht="17.25">
+    <row r="56" spans="1:14" ht="17.5">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="5"/>
@@ -5003,7 +5340,7 @@
       <c r="M56" s="5"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:14" ht="17.25">
+    <row r="57" spans="1:14" ht="17.5">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="5"/>
@@ -5011,7 +5348,7 @@
       <c r="M57" s="4"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" ht="17.25">
+    <row r="58" spans="1:14" ht="17.5">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="5"/>
@@ -5019,14 +5356,14 @@
       <c r="M58" s="4"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" ht="17.25">
+    <row r="59" spans="1:14" ht="17.5">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="C59" s="5"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="17.25">
+    <row r="60" spans="1:14" ht="17.5">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="5"/>
@@ -5075,15 +5412,15 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G16" sqref="G9:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" customWidth="1"/>
     <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.08203125" style="3" customWidth="1"/>
     <col min="8" max="10" width="9" style="8"/>
   </cols>
   <sheetData>
@@ -6307,4 +6644,1738 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A065B9-8F8B-44F0-9CC5-4E2126586474}">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H20:H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>2.7159965104290587</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>2.7159965104290587</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>5.19</v>
+      </c>
+      <c r="C3">
+        <v>6.2</v>
+      </c>
+      <c r="D3">
+        <v>6.8</v>
+      </c>
+      <c r="E3">
+        <v>1.94</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1.8303941908713692</v>
+      </c>
+      <c r="G3" s="3">
+        <f>1-E3/F3</f>
+        <v>-5.9880986115046664E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>1.94</v>
+      </c>
+      <c r="L3" s="10">
+        <v>1.8303941908713692</v>
+      </c>
+      <c r="M3" s="3">
+        <f>1-K3/L3</f>
+        <v>-5.9880986115046664E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>5.73</v>
+      </c>
+      <c r="C4">
+        <v>5.85</v>
+      </c>
+      <c r="D4">
+        <v>7.32</v>
+      </c>
+      <c r="E4">
+        <v>2.23</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2.4171860019175457</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G12" si="0">1-E4/F4</f>
+        <v>7.7439635083544123E-2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>2.23</v>
+      </c>
+      <c r="L4" s="10">
+        <v>2.4171860019175457</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M9" si="1">1-K4/L4</f>
+        <v>7.7439635083544123E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>5.74</v>
+      </c>
+      <c r="C5">
+        <v>5.72</v>
+      </c>
+      <c r="D5">
+        <v>7.6</v>
+      </c>
+      <c r="E5">
+        <v>2.33</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.3622394784073841</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3647845064853392E-2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <v>2.33</v>
+      </c>
+      <c r="L5" s="10">
+        <v>2.3622394784073841</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3647845064853392E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>5.62</v>
+      </c>
+      <c r="C6">
+        <v>5.58</v>
+      </c>
+      <c r="D6">
+        <v>7.73</v>
+      </c>
+      <c r="E6">
+        <v>2.39</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2.4381945777607132</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9766501902803824E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6">
+        <v>2.39</v>
+      </c>
+      <c r="L6" s="10">
+        <v>2.4381945777607132</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.9766501902803824E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>5.39</v>
+      </c>
+      <c r="C7">
+        <v>5.36</v>
+      </c>
+      <c r="D7">
+        <v>7.7</v>
+      </c>
+      <c r="E7">
+        <v>2.44</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2.6302056835525836</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.231589709580255E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7">
+        <v>2.44</v>
+      </c>
+      <c r="L7" s="10">
+        <v>2.6302056835525836</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="1"/>
+        <v>7.231589709580255E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="C8">
+        <v>4.99</v>
+      </c>
+      <c r="D8">
+        <v>7.57</v>
+      </c>
+      <c r="E8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2.5056768558951963</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7253398396654962E-3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L8" s="10">
+        <v>2.5056768558951963</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.7253398396654962E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>4.66</v>
+      </c>
+      <c r="C9">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D9">
+        <v>7.31</v>
+      </c>
+      <c r="E9">
+        <v>2.58</v>
+      </c>
+      <c r="F9" s="10">
+        <v>2.6201923076923075</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.53394495412843E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9">
+        <v>2.58</v>
+      </c>
+      <c r="L9" s="10">
+        <v>2.6201923076923075</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.53394495412843E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C10">
+        <v>4.58</v>
+      </c>
+      <c r="D10">
+        <v>7.28</v>
+      </c>
+      <c r="E10">
+        <v>2.59</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10">
+        <v>2.59</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11">
+        <v>4.53</v>
+      </c>
+      <c r="C11">
+        <v>4.54</v>
+      </c>
+      <c r="D11">
+        <v>7.38</v>
+      </c>
+      <c r="E11">
+        <v>2.63</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <v>2.63</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>1448</v>
+      </c>
+      <c r="B15">
+        <v>17367</v>
+      </c>
+      <c r="C15">
+        <v>54472</v>
+      </c>
+      <c r="D15">
+        <v>49565</v>
+      </c>
+      <c r="E15">
+        <v>15247</v>
+      </c>
+      <c r="F15">
+        <v>3884</v>
+      </c>
+      <c r="G15">
+        <v>275</v>
+      </c>
+      <c r="H15">
+        <v>39669</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>2081</v>
+      </c>
+      <c r="B16">
+        <v>22971</v>
+      </c>
+      <c r="C16">
+        <v>74511</v>
+      </c>
+      <c r="D16">
+        <v>64740</v>
+      </c>
+      <c r="E16">
+        <v>20942</v>
+      </c>
+      <c r="F16">
+        <v>4723</v>
+      </c>
+      <c r="G16">
+        <v>270</v>
+      </c>
+      <c r="H16">
+        <v>63069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1928</v>
+      </c>
+      <c r="B17">
+        <v>16688</v>
+      </c>
+      <c r="C17">
+        <v>54602</v>
+      </c>
+      <c r="D17">
+        <v>46881</v>
+      </c>
+      <c r="E17">
+        <v>13759</v>
+      </c>
+      <c r="F17">
+        <v>3435</v>
+      </c>
+      <c r="G17">
+        <v>208</v>
+      </c>
+      <c r="H17">
+        <v>37827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <f>(A15+A16)/A17</f>
+        <v>1.8303941908713692</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:H18" si="2">(B15+B16)/B17</f>
+        <v>2.4171860019175457</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>2.3622394784073841</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>2.4381945777607132</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>2.6302056835525836</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>2.5056768558951963</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>2.6201923076923075</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>2.7159965104290587</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>267</v>
+      </c>
+      <c r="B19">
+        <v>2625</v>
+      </c>
+      <c r="C19">
+        <v>8242</v>
+      </c>
+      <c r="D19">
+        <v>7205</v>
+      </c>
+      <c r="E19">
+        <v>2154</v>
+      </c>
+      <c r="F19">
+        <v>530</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>5410</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <f>A15/$A$19</f>
+        <v>5.4232209737827715</v>
+      </c>
+      <c r="B20">
+        <f>B15/B$19</f>
+        <v>6.6159999999999997</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:H20" si="3">C15/C$19</f>
+        <v>6.6090754671196308</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>6.8792505204718948</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>7.0784586815227488</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>7.3283018867924525</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>7.3325323475046211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <f t="shared" ref="A21:H22" si="4">A16/$A$19</f>
+        <v>7.7940074906367043</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:H22" si="5">B16/B$19</f>
+        <v>8.7508571428571429</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="5"/>
+        <v>9.0404028148507649</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>8.9854267869535054</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>9.7223769730733522</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>8.9113207547169804</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>11.657855822550832</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <f t="shared" si="4"/>
+        <v>7.2209737827715355</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="5"/>
+        <v>6.3573333333333331</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="5"/>
+        <v>6.6248483377820921</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="5"/>
+        <v>6.5067314365024291</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>6.3876508820798517</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>6.4811320754716979</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>6.9333333333333336</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="5"/>
+        <v>6.9920517560073936</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14AE4EB-220C-404D-BDD7-5A155A787AB6}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="A14:J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="2" max="4" width="8.6640625" style="8"/>
+    <col min="7" max="9" width="8.6640625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>39669</v>
+      </c>
+      <c r="C2" s="8">
+        <v>63069</v>
+      </c>
+      <c r="D2" s="8">
+        <v>37827</v>
+      </c>
+      <c r="F2">
+        <v>5410</v>
+      </c>
+      <c r="G2" s="10">
+        <f>B2/$F2</f>
+        <v>7.3325323475046211</v>
+      </c>
+      <c r="H2" s="10">
+        <f>C2/$F2</f>
+        <v>11.657855822550832</v>
+      </c>
+      <c r="I2" s="10">
+        <f>D2/$F2</f>
+        <v>6.9920517560073936</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10">
+        <v>2.7159965104290587</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1448</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2081</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1928</v>
+      </c>
+      <c r="F3">
+        <v>267</v>
+      </c>
+      <c r="G3" s="10">
+        <f>B3/$F$3</f>
+        <v>5.4232209737827715</v>
+      </c>
+      <c r="H3" s="10">
+        <f>C3/$F$3</f>
+        <v>7.7940074906367043</v>
+      </c>
+      <c r="I3" s="10">
+        <f>D3/$F$3</f>
+        <v>7.2209737827715355</v>
+      </c>
+      <c r="J3">
+        <v>1.94</v>
+      </c>
+      <c r="K3" s="10">
+        <v>1.8303941908713692</v>
+      </c>
+      <c r="L3" s="3">
+        <f>1-J3/K3</f>
+        <v>-5.9880986115046664E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>17367</v>
+      </c>
+      <c r="C4" s="8">
+        <v>22971</v>
+      </c>
+      <c r="D4" s="8">
+        <v>16688</v>
+      </c>
+      <c r="F4">
+        <v>2625</v>
+      </c>
+      <c r="G4" s="10">
+        <f>B4/$F4</f>
+        <v>6.6159999999999997</v>
+      </c>
+      <c r="H4" s="10">
+        <f>C4/$F4</f>
+        <v>8.7508571428571429</v>
+      </c>
+      <c r="I4" s="10">
+        <f>D4/$F4</f>
+        <v>6.3573333333333331</v>
+      </c>
+      <c r="J4">
+        <v>2.23</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2.4171860019175457</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L9" si="0">1-J4/K4</f>
+        <v>7.7439635083544123E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>54472</v>
+      </c>
+      <c r="C5" s="8">
+        <v>74511</v>
+      </c>
+      <c r="D5" s="8">
+        <v>54602</v>
+      </c>
+      <c r="F5">
+        <v>8242</v>
+      </c>
+      <c r="G5" s="10">
+        <f>B5/$F5</f>
+        <v>6.6090754671196308</v>
+      </c>
+      <c r="H5" s="10">
+        <f>C5/$F5</f>
+        <v>9.0404028148507649</v>
+      </c>
+      <c r="I5" s="10">
+        <f>D5/$F5</f>
+        <v>6.6248483377820921</v>
+      </c>
+      <c r="J5">
+        <v>2.33</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2.3622394784073841</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3647845064853392E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>49565</v>
+      </c>
+      <c r="C6" s="8">
+        <v>64740</v>
+      </c>
+      <c r="D6" s="8">
+        <v>46881</v>
+      </c>
+      <c r="F6">
+        <v>7205</v>
+      </c>
+      <c r="G6" s="10">
+        <f>B6/$F6</f>
+        <v>6.8792505204718948</v>
+      </c>
+      <c r="H6" s="10">
+        <f>C6/$F6</f>
+        <v>8.9854267869535054</v>
+      </c>
+      <c r="I6" s="10">
+        <f>D6/$F6</f>
+        <v>6.5067314365024291</v>
+      </c>
+      <c r="J6">
+        <v>2.39</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2.4381945777607132</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9766501902803824E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>15247</v>
+      </c>
+      <c r="C7" s="8">
+        <v>20942</v>
+      </c>
+      <c r="D7" s="8">
+        <v>13759</v>
+      </c>
+      <c r="F7">
+        <v>2154</v>
+      </c>
+      <c r="G7" s="10">
+        <f>B7/$F7</f>
+        <v>7.0784586815227488</v>
+      </c>
+      <c r="H7" s="10">
+        <f>C7/$F7</f>
+        <v>9.7223769730733522</v>
+      </c>
+      <c r="I7" s="10">
+        <f>D7/$F7</f>
+        <v>6.3876508820798517</v>
+      </c>
+      <c r="J7">
+        <v>2.44</v>
+      </c>
+      <c r="K7" s="10">
+        <v>2.6302056835525836</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.231589709580255E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3884</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4723</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3435</v>
+      </c>
+      <c r="F8">
+        <v>530</v>
+      </c>
+      <c r="G8" s="10">
+        <f>B8/$F8</f>
+        <v>7.3283018867924525</v>
+      </c>
+      <c r="H8" s="10">
+        <f>C8/$F8</f>
+        <v>8.9113207547169804</v>
+      </c>
+      <c r="I8" s="10">
+        <f>D8/$F8</f>
+        <v>6.4811320754716979</v>
+      </c>
+      <c r="J8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="K8" s="10">
+        <v>2.5056768558951963</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7253398396654962E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>275</v>
+      </c>
+      <c r="C9" s="8">
+        <v>270</v>
+      </c>
+      <c r="D9" s="8">
+        <v>208</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9" s="10">
+        <f>B9/$F9</f>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="H9" s="10">
+        <f>C9/$F9</f>
+        <v>9</v>
+      </c>
+      <c r="I9" s="10">
+        <f>D9/$F9</f>
+        <v>6.9333333333333336</v>
+      </c>
+      <c r="J9">
+        <v>2.58</v>
+      </c>
+      <c r="K9" s="10">
+        <v>2.6201923076923075</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.53394495412843E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10">
+        <v>2.59</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11">
+        <v>2.63</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="11">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="12">
+        <v>7.3325323475046211</v>
+      </c>
+      <c r="C15" s="12">
+        <v>6.9920517560073936</v>
+      </c>
+      <c r="D15" s="12">
+        <v>11.657855822550832</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>2.7159965104290587</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="12">
+        <v>5.4232209737827715</v>
+      </c>
+      <c r="C16" s="12">
+        <v>7.2209737827715355</v>
+      </c>
+      <c r="D16" s="12">
+        <v>7.7940074906367043</v>
+      </c>
+      <c r="E16">
+        <v>5.19</v>
+      </c>
+      <c r="F16">
+        <v>6.2</v>
+      </c>
+      <c r="G16">
+        <v>6.8</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1.8303941908713692</v>
+      </c>
+      <c r="I16">
+        <v>1.94</v>
+      </c>
+      <c r="J16" s="3">
+        <f>1-I16/H16</f>
+        <v>-5.9880986115046664E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="12">
+        <v>6.6159999999999997</v>
+      </c>
+      <c r="C17" s="12">
+        <v>6.3573333333333331</v>
+      </c>
+      <c r="D17" s="12">
+        <v>8.7508571428571429</v>
+      </c>
+      <c r="E17">
+        <v>5.73</v>
+      </c>
+      <c r="F17">
+        <v>5.85</v>
+      </c>
+      <c r="G17">
+        <v>7.32</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2.4171860019175457</v>
+      </c>
+      <c r="I17">
+        <v>2.23</v>
+      </c>
+      <c r="J17" s="3">
+        <f>1-I17/H17</f>
+        <v>7.7439635083544123E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="12">
+        <v>6.6090754671196308</v>
+      </c>
+      <c r="C18" s="12">
+        <v>6.6248483377820921</v>
+      </c>
+      <c r="D18" s="12">
+        <v>9.0404028148507649</v>
+      </c>
+      <c r="E18">
+        <v>5.74</v>
+      </c>
+      <c r="F18">
+        <v>5.72</v>
+      </c>
+      <c r="G18">
+        <v>7.6</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2.3622394784073841</v>
+      </c>
+      <c r="I18">
+        <v>2.33</v>
+      </c>
+      <c r="J18" s="3">
+        <f>1-I18/H18</f>
+        <v>1.3647845064853392E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12">
+        <v>6.8792505204718948</v>
+      </c>
+      <c r="C19" s="12">
+        <v>6.5067314365024291</v>
+      </c>
+      <c r="D19" s="12">
+        <v>8.9854267869535054</v>
+      </c>
+      <c r="E19">
+        <v>5.62</v>
+      </c>
+      <c r="F19">
+        <v>5.58</v>
+      </c>
+      <c r="G19">
+        <v>7.73</v>
+      </c>
+      <c r="H19" s="10">
+        <v>2.4381945777607132</v>
+      </c>
+      <c r="I19">
+        <v>2.39</v>
+      </c>
+      <c r="J19" s="3">
+        <f>1-I19/H19</f>
+        <v>1.9766501902803824E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="12">
+        <v>7.0784586815227488</v>
+      </c>
+      <c r="C20" s="12">
+        <v>6.3876508820798517</v>
+      </c>
+      <c r="D20" s="12">
+        <v>9.7223769730733522</v>
+      </c>
+      <c r="E20">
+        <v>5.39</v>
+      </c>
+      <c r="F20">
+        <v>5.36</v>
+      </c>
+      <c r="G20">
+        <v>7.7</v>
+      </c>
+      <c r="H20" s="10">
+        <v>2.6302056835525836</v>
+      </c>
+      <c r="I20">
+        <v>2.44</v>
+      </c>
+      <c r="J20" s="3">
+        <f>1-I20/H20</f>
+        <v>7.231589709580255E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="12">
+        <v>7.3283018867924525</v>
+      </c>
+      <c r="C21" s="12">
+        <v>6.4811320754716979</v>
+      </c>
+      <c r="D21" s="12">
+        <v>8.9113207547169804</v>
+      </c>
+      <c r="E21">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F21">
+        <v>4.99</v>
+      </c>
+      <c r="G21">
+        <v>7.57</v>
+      </c>
+      <c r="H21" s="10">
+        <v>2.5056768558951963</v>
+      </c>
+      <c r="I21">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J21" s="3">
+        <f>1-I21/H21</f>
+        <v>-1.7253398396654962E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="12">
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="C22" s="12">
+        <v>6.9333333333333336</v>
+      </c>
+      <c r="D22" s="12">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>4.66</v>
+      </c>
+      <c r="F22">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G22">
+        <v>7.31</v>
+      </c>
+      <c r="H22" s="10">
+        <v>2.6201923076923075</v>
+      </c>
+      <c r="I22">
+        <v>2.58</v>
+      </c>
+      <c r="J22" s="3">
+        <f>1-I22/H22</f>
+        <v>1.53394495412843E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F23">
+        <v>4.58</v>
+      </c>
+      <c r="G23">
+        <v>7.28</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>2.59</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>4.53</v>
+      </c>
+      <c r="F24">
+        <v>4.54</v>
+      </c>
+      <c r="G24">
+        <v>7.38</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>2.63</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="H25"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G3:I3" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510546F1-4A98-46AB-8EA1-5DA1426B4607}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="2" max="2" width="8.6640625" style="2"/>
+    <col min="4" max="5" width="8.6640625" style="8"/>
+    <col min="6" max="6" width="8.6640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="13">
+        <v>7281</v>
+      </c>
+      <c r="E3" s="13">
+        <v>7813</v>
+      </c>
+      <c r="F3" s="17">
+        <f>D3/(D3+E3)</f>
+        <v>0.48237710348482843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1118</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1023</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" ref="F4:F12" si="0">D4/(D4+E4)</f>
+        <v>0.5221858944418496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1236</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1238</v>
+      </c>
+      <c r="F5" s="17">
+        <f t="shared" si="0"/>
+        <v>0.49959579628132578</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="13">
+        <v>2567</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2579</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>0.49883404586086283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="13">
+        <v>680</v>
+      </c>
+      <c r="E7" s="13">
+        <v>694</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="0"/>
+        <v>0.49490538573508008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="13">
+        <v>113</v>
+      </c>
+      <c r="E8" s="13">
+        <v>121</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.48290598290598291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="8">
+        <f>SUM(D3:D4)</f>
+        <v>8399</v>
+      </c>
+      <c r="E9" s="8">
+        <f>SUM(E3:E4)</f>
+        <v>8836</v>
+      </c>
+      <c r="F9" s="17">
+        <f>D9/(D9+E9)</f>
+        <v>0.48732230925442416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="8">
+        <f>SUM(D5:D6)</f>
+        <v>3803</v>
+      </c>
+      <c r="E10" s="8">
+        <f>SUM(E5:E6)</f>
+        <v>3817</v>
+      </c>
+      <c r="F10" s="17">
+        <f>D10/(D10+E10)</f>
+        <v>0.4990813648293963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="8">
+        <f>SUM(D7:D8)</f>
+        <v>793</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E7:E8)</f>
+        <v>815</v>
+      </c>
+      <c r="F11" s="17">
+        <f>D11/(D11+E11)</f>
+        <v>0.49315920398009949</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="8">
+        <f>SUM(D3:D8)</f>
+        <v>12995</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E3:E8)</f>
+        <v>13468</v>
+      </c>
+      <c r="F12" s="17">
+        <f>D12/(D12+E12)</f>
+        <v>0.4910629936137248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>